<commit_message>
table of contents formatting
</commit_message>
<xml_diff>
--- a/docs/user-guide/Network_NAD_VLAN_Mapping-Example.xlsx
+++ b/docs/user-guide/Network_NAD_VLAN_Mapping-Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fwardzic/Documents/00-Noiro-work/!CNO Airtel/cko/docs/user-guide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE379CE-F85D-F946-A90C-EC93D9ACA3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B07667F-0506-1442-A8F9-2698C39B7576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13400" yWindow="34600" windowWidth="34560" windowHeight="19980" xr2:uid="{465B9B70-6C4A-FC48-8E91-44046C1C1C8C}"/>
   </bookViews>
@@ -661,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F28E309-79A1-5A4B-A9BE-82B5E1048504}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>